<commit_message>
parser works, db part still needed
</commit_message>
<xml_diff>
--- a/B_report.xlsx
+++ b/B_report.xlsx
@@ -25,31 +25,31 @@
     <t>Version</t>
   </si>
   <si>
-    <t>Loren</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>Velasquez</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
     <t>Job</t>
   </si>
   <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Data Engineer</t>
+  </si>
+  <si>
+    <t>Tiberius</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -497,30 +497,30 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>812</v>
@@ -528,16 +528,16 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>

</xml_diff>